<commit_message>
excel con la caja mágica
</commit_message>
<xml_diff>
--- a/T1/Datos.xlsx
+++ b/T1/Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiegoYera\Desktop\2025-2\Econo_Med\Tareas_Economed\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A96DD0-AB87-402A-ADB1-4BB0DC48B6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A56D935-00B9-43F0-90FA-80EA2C84B0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="733" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="733" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Centrales" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="156">
   <si>
     <t>Potencia</t>
   </si>
@@ -526,6 +526,30 @@
   </si>
   <si>
     <t>pasar a MW</t>
+  </si>
+  <si>
+    <t>Caja Mágica</t>
+  </si>
+  <si>
+    <t>Entran GWh</t>
+  </si>
+  <si>
+    <t>Salen Ton</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>cc-gnl</t>
+  </si>
+  <si>
+    <t>GWh -&gt; KWh</t>
+  </si>
+  <si>
+    <t>1Millon</t>
+  </si>
+  <si>
+    <t>carbon</t>
   </si>
 </sst>
 </file>
@@ -597,7 +621,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -623,12 +647,222 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -713,6 +947,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3012,14 +3273,15 @@
   </sheetPr>
   <dimension ref="A2:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.85546875" style="13" customWidth="1"/>
-    <col min="8" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3060,7 +3322,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>53</v>
       </c>
@@ -3099,7 +3361,9 @@
         <v>144</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="15"/>
+      <c r="J8" s="54" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
@@ -3118,9 +3382,11 @@
         <v>3163.160948187648</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J9" s="55">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>56</v>
       </c>
@@ -3137,7 +3403,9 @@
         <v>3163.160948187648</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="15"/>
+      <c r="J10" s="56" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="13" t="s">
@@ -3177,7 +3445,7 @@
       <c r="I12" s="13"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="15"/>
@@ -3187,10 +3455,21 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H14" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="I14" s="44"/>
+    </row>
+    <row r="15" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
         <v>70</v>
+      </c>
+      <c r="G15" s="41"/>
+      <c r="H15" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
@@ -3198,8 +3477,18 @@
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="50">
+        <v>1</v>
+      </c>
+      <c r="I16" s="51">
+        <f>H16*J9*D35*(1/C18)*C26*(1/1000)</f>
+        <v>79.680815196650229</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="14"/>
       <c r="C17" s="21" t="s">
         <v>72</v>
@@ -3210,8 +3499,19 @@
       <c r="E17" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="48"/>
+      <c r="G17" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" s="42">
+        <v>1</v>
+      </c>
+      <c r="I17" s="45">
+        <f>H17*J9*D35*(1/C20)*C27*(1/1000)</f>
+        <v>61.960311166384507</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>71</v>
       </c>
@@ -3220,8 +3520,18 @@
         <v>9120000</v>
       </c>
       <c r="D18" s="19"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="H18" s="46">
+        <v>1</v>
+      </c>
+      <c r="I18" s="47">
+        <f>H18*J9*D35*(1/D19)*(1/1000)</f>
+        <v>132.3056958750023</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="13" t="s">
         <v>73</v>
       </c>
@@ -3229,8 +3539,9 @@
       <c r="D19" s="19">
         <v>6500</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="48"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>43</v>
       </c>
@@ -3239,29 +3550,29 @@
       </c>
       <c r="D20" s="19"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="16" t="s">
         <v>80</v>
       </c>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="14"/>
       <c r="C25" s="21" t="s">
         <v>77</v>
@@ -3270,7 +3581,7 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
         <v>71</v>
       </c>
@@ -3281,7 +3592,7 @@
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>43</v>
       </c>
@@ -3291,12 +3602,12 @@
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>75</v>
       </c>
@@ -3420,6 +3731,9 @@
       <c r="A57" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H14:I14"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3969,7 +4283,7 @@
   <dimension ref="B2:Q44"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
mira, tira cualquier cosa esta caga de modelo
</commit_message>
<xml_diff>
--- a/T1/Datos.xlsx
+++ b/T1/Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiegoYera\Desktop\2025-2\Econo_Med\Tareas_Economed\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B9935F-72DB-4546-9167-C2D8BA942641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C539582-D5FD-4525-AD28-06D0AB457153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="29040" windowHeight="15720" tabRatio="733" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="733" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Centrales" sheetId="1" r:id="rId1"/>
@@ -1168,7 +1168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1323,6 +1323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1633,8 +1634,8 @@
   </sheetPr>
   <dimension ref="A2:O65540"/>
   <sheetViews>
-    <sheetView topLeftCell="B52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70:N70"/>
+    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1772,8 +1773,8 @@
         <f>J8+H8+F8</f>
         <v>48.7</v>
       </c>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
       <c r="N8" t="s">
         <v>15</v>
       </c>
@@ -1808,8 +1809,8 @@
         <f t="shared" ref="K9:K28" si="0">J9+H9+F9</f>
         <v>44.5</v>
       </c>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
       <c r="N9" s="23" t="s">
         <v>135</v>
       </c>
@@ -2677,10 +2678,10 @@
       <c r="K46" s="6">
         <v>2030</v>
       </c>
-      <c r="L46" t="s">
+      <c r="L46" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="M46" s="24" t="s">
+      <c r="M46" s="27" t="s">
         <v>142</v>
       </c>
       <c r="N46" s="6" t="s">
@@ -4392,7 +4393,7 @@
   <dimension ref="A2:J57"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:F12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5401,8 +5402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
1.1_ hay que hacer cambios de cantidades
</commit_message>
<xml_diff>
--- a/T1/Datos.xlsx
+++ b/T1/Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiegoYera\Desktop\2025-2\Econo_Med\Tareas_Economed\T1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/dpgarces_uc_cl/Documents/Universidad/2025-2/Econo&amp;Med/Tareas_Economed/T1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C539582-D5FD-4525-AD28-06D0AB457153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1C539582-D5FD-4525-AD28-06D0AB457153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A30C3D20-7D50-4704-AD38-58453FF8ABB4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="733" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3312" yWindow="3312" windowWidth="17280" windowHeight="8880" tabRatio="733" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Centrales" sheetId="1" r:id="rId1"/>
@@ -1168,7 +1168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1323,7 +1323,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1634,30 +1633,30 @@
   </sheetPr>
   <dimension ref="A2:O65540"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="F1" zoomScale="127" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>90</v>
       </c>
@@ -1665,7 +1664,7 @@
         <v>3412</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1686,7 +1685,7 @@
       </c>
       <c r="K4" s="33"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1706,7 +1705,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
         <v>100</v>
       </c>
@@ -1738,7 +1737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
@@ -1746,7 +1745,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="55">
         <v>1</v>
       </c>
@@ -1773,8 +1772,6 @@
         <f>J8+H8+F8</f>
         <v>48.7</v>
       </c>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
       <c r="N8" t="s">
         <v>15</v>
       </c>
@@ -1782,7 +1779,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="55">
         <v>2</v>
       </c>
@@ -1809,8 +1806,6 @@
         <f t="shared" ref="K9:K28" si="0">J9+H9+F9</f>
         <v>44.5</v>
       </c>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76"/>
       <c r="N9" s="23" t="s">
         <v>135</v>
       </c>
@@ -1818,7 +1813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="55">
         <v>3</v>
       </c>
@@ -1860,7 +1855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="55">
         <v>4</v>
       </c>
@@ -1896,7 +1891,7 @@
         <v>27.471428571428575</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="55">
         <v>5</v>
       </c>
@@ -1932,7 +1927,7 @@
         <v>26.547368421052632</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="55">
         <v>6</v>
       </c>
@@ -1968,7 +1963,7 @@
         <v>63.523348017621146</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="55">
         <v>7</v>
       </c>
@@ -2004,7 +1999,7 @@
         <v>169.91428571428571</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="55">
         <v>8</v>
       </c>
@@ -2040,7 +2035,7 @@
         <v>148.90597014925373</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="55">
         <v>9</v>
       </c>
@@ -2076,7 +2071,7 @@
         <v>136.39944134078212</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="55">
         <v>10</v>
       </c>
@@ -2112,7 +2107,7 @@
         <v>212.30588235294118</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="55">
         <v>11</v>
       </c>
@@ -2148,7 +2143,7 @@
         <v>168.95424836601308</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="55">
         <v>12</v>
       </c>
@@ -2184,7 +2179,7 @@
         <v>114.88280098280099</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="55">
         <v>13</v>
       </c>
@@ -2220,7 +2215,7 @@
         <v>223.53137254901961</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="55">
         <v>14</v>
       </c>
@@ -2256,7 +2251,7 @@
         <v>162.1142857142857</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="55">
         <v>15</v>
       </c>
@@ -2292,7 +2287,7 @@
         <v>174.15395683453238</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="55">
         <v>16</v>
       </c>
@@ -2328,7 +2323,7 @@
         <v>132.15431754874652</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="55">
         <v>17</v>
       </c>
@@ -2364,7 +2359,7 @@
         <v>153.45135135135135</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="55">
         <v>18</v>
       </c>
@@ -2400,7 +2395,7 @@
         <v>143.86980609418282</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="55">
         <v>19</v>
       </c>
@@ -2426,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="55">
         <v>20</v>
       </c>
@@ -2454,7 +2449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="55">
         <v>21</v>
       </c>
@@ -2482,7 +2477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="55">
         <v>22</v>
       </c>
@@ -2510,22 +2505,22 @@
         <v>500</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D33" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>12</v>
       </c>
@@ -2534,7 +2529,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>15</v>
       </c>
@@ -2543,7 +2538,7 @@
         <v>2193</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>19</v>
       </c>
@@ -2552,7 +2547,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>20</v>
       </c>
@@ -2561,7 +2556,7 @@
         <v>3556</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>29</v>
       </c>
@@ -2570,7 +2565,7 @@
         <v>5571</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>30</v>
       </c>
@@ -2579,7 +2574,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" s="23" t="s">
         <v>39</v>
       </c>
@@ -2588,11 +2583,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" s="23"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>6</v>
       </c>
@@ -2601,7 +2596,7 @@
         <v>12707</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>33</v>
       </c>
@@ -2612,7 +2607,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D45" s="3" t="s">
         <v>34</v>
       </c>
@@ -2647,7 +2642,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="25" t="s">
         <v>100</v>
       </c>
@@ -2688,7 +2683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -2733,7 +2728,7 @@
         <v>34.44736842105263</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -2778,7 +2773,7 @@
         <v>29.447368421052634</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2823,7 +2818,7 @@
         <v>24.747368421052634</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
@@ -2868,7 +2863,7 @@
         <v>24.747368421052634</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2913,7 +2908,7 @@
         <v>27.447368421052634</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6</v>
       </c>
@@ -2958,7 +2953,7 @@
         <v>29.447368421052634</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7</v>
       </c>
@@ -3003,7 +2998,7 @@
         <v>64.357777777777784</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>37</v>
       </c>
@@ -3011,7 +3006,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>8</v>
       </c>
@@ -3048,10 +3043,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K57" s="24"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9</v>
       </c>
@@ -3090,7 +3085,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>10</v>
       </c>
@@ -3129,7 +3124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>11</v>
       </c>
@@ -3168,7 +3163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>12</v>
       </c>
@@ -3207,7 +3202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>13</v>
       </c>
@@ -3246,7 +3241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>14</v>
       </c>
@@ -3285,11 +3280,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J64" s="9"/>
       <c r="N64" s="8"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>15</v>
       </c>
@@ -3335,7 +3330,7 @@
         <v>169.85333333333332</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>16</v>
       </c>
@@ -3381,7 +3376,7 @@
         <v>164.85333333333332</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>17</v>
       </c>
@@ -3427,7 +3422,7 @@
         <v>160.15333333333334</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>18</v>
       </c>
@@ -3473,7 +3468,7 @@
         <v>160.15333333333334</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>19</v>
       </c>
@@ -3519,7 +3514,7 @@
         <v>162.85333333333332</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>20</v>
       </c>
@@ -3565,17 +3560,17 @@
         <v>164.85333333333332</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E71" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B73" s="23" t="s">
         <v>101</v>
       </c>
@@ -3584,12 +3579,12 @@
       </c>
       <c r="E73" s="36"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65540" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="65540" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K65540" s="11" t="s">
         <v>37</v>
       </c>
@@ -3613,19 +3608,19 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C6" s="24" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -3633,7 +3628,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>135</v>
       </c>
@@ -3641,7 +3636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>43</v>
       </c>
@@ -3649,7 +3644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>101</v>
       </c>
@@ -3672,9 +3667,9 @@
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>47</v>
       </c>
@@ -3685,7 +3680,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="6" t="s">
         <v>48</v>
@@ -3697,7 +3692,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>44</v>
       </c>
@@ -3712,7 +3707,7 @@
         <v>9307.2000000000007</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>45</v>
       </c>
@@ -3727,7 +3722,7 @@
         <v>24770.831999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>46</v>
       </c>
@@ -3742,10 +3737,10 @@
         <v>16266.384</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8">
         <f>+SUM(C4:C6)</f>
         <v>8760</v>
@@ -3755,7 +3750,7 @@
         <v>50344.415999999997</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="70" t="s">
         <v>232</v>
       </c>
@@ -3771,7 +3766,7 @@
       <c r="L11" s="70"/>
       <c r="M11" s="70"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>86</v>
       </c>
@@ -3797,7 +3792,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="20">
         <v>2017</v>
       </c>
@@ -3835,7 +3830,7 @@
         <v>4868.46</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="20">
         <v>2018</v>
       </c>
@@ -3875,7 +3870,7 @@
         <v>4965.8292000000001</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="20">
         <v>2019</v>
       </c>
@@ -3915,7 +3910,7 @@
         <v>5065.1457840000003</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="20">
         <v>2020</v>
       </c>
@@ -3955,7 +3950,7 @@
         <v>5166.4486996800006</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="20">
         <v>2021</v>
       </c>
@@ -3995,7 +3990,7 @@
         <v>5269.7776736736005</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="20">
         <v>2022</v>
       </c>
@@ -4035,7 +4030,7 @@
         <v>5375.1732271470728</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="20">
         <v>2023</v>
       </c>
@@ -4075,7 +4070,7 @@
         <v>5482.6766916900142</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="20">
         <v>2024</v>
       </c>
@@ -4115,7 +4110,7 @@
         <v>5592.330225523815</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="20">
         <v>2025</v>
       </c>
@@ -4155,7 +4150,7 @@
         <v>5704.176830034291</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="20">
         <v>2026</v>
       </c>
@@ -4195,7 +4190,7 @@
         <v>5818.2603666349769</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="20">
         <v>2027</v>
       </c>
@@ -4235,7 +4230,7 @@
         <v>5934.6255739676762</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="20">
         <v>2028</v>
       </c>
@@ -4275,7 +4270,7 @@
         <v>6053.3180854470302</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="20">
         <v>2029</v>
       </c>
@@ -4315,7 +4310,7 @@
         <v>6174.3844471559705</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="20">
         <v>2030</v>
       </c>
@@ -4355,7 +4350,7 @@
         <v>24403.759722847823</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K27">
         <f>K26*C4</f>
         <v>12280652.743578767</v>
@@ -4393,23 +4388,23 @@
   <dimension ref="A2:J57"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>59</v>
       </c>
@@ -4426,7 +4421,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="6" t="s">
         <v>52</v>
@@ -4441,7 +4436,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>53</v>
       </c>
@@ -4460,7 +4455,7 @@
       <c r="I7" s="12"/>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>54</v>
       </c>
@@ -4484,7 +4479,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>55</v>
       </c>
@@ -4505,7 +4500,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>56</v>
       </c>
@@ -4526,7 +4521,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>57</v>
       </c>
@@ -4545,7 +4540,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>58</v>
       </c>
@@ -4564,13 +4559,13 @@
       <c r="I12" s="12"/>
       <c r="J12" s="14"/>
     </row>
-    <row r="13" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -4579,7 +4574,7 @@
       </c>
       <c r="I14" s="72"/>
     </row>
-    <row r="15" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
         <v>70</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -4607,7 +4602,7 @@
         <v>79.680815196650229</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="19" t="s">
         <v>72</v>
@@ -4629,7 +4624,7 @@
         <v>61.960311166384507</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
         <v>71</v>
       </c>
@@ -4649,7 +4644,7 @@
         <v>132.3056958750023</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>73</v>
       </c>
@@ -4658,7 +4653,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>43</v>
       </c>
@@ -4667,29 +4662,29 @@
       </c>
       <c r="D20" s="17"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
         <v>80</v>
       </c>
       <c r="F23" s="16"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="13"/>
       <c r="C25" s="19" t="s">
         <v>77</v>
@@ -4698,7 +4693,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>71</v>
       </c>
@@ -4709,7 +4704,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>43</v>
       </c>
@@ -4719,12 +4714,12 @@
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>75</v>
       </c>
@@ -4738,7 +4733,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>75</v>
       </c>
@@ -4753,7 +4748,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>84</v>
       </c>
@@ -4768,7 +4763,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>85</v>
       </c>
@@ -4783,7 +4778,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>79</v>
       </c>
@@ -4797,7 +4792,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="22" t="s">
         <v>89</v>
       </c>
@@ -4808,43 +4803,43 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
     </row>
   </sheetData>
@@ -4862,26 +4857,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:K90"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B4" s="12"/>
       <c r="C4" s="3" t="s">
         <v>50</v>
@@ -4896,7 +4891,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="27" t="s">
         <v>106</v>
@@ -4911,7 +4906,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -4931,7 +4926,7 @@
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -4951,7 +4946,7 @@
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -4971,7 +4966,7 @@
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>24</v>
       </c>
@@ -4991,7 +4986,7 @@
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -5011,7 +5006,7 @@
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -5031,7 +5026,7 @@
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -5051,7 +5046,7 @@
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -5071,7 +5066,7 @@
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -5091,7 +5086,7 @@
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -5111,7 +5106,7 @@
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -5131,7 +5126,7 @@
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>27</v>
       </c>
@@ -5151,7 +5146,7 @@
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -5171,226 +5166,226 @@
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="28" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="28" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="23" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="12"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="12"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="12"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="12"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="12"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="12"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="12"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="12"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="12"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="12"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="12"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="12"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="12"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="12"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="12"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="12"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="12"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="12"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="12"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="12"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="12"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="12"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="12"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="12"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="12"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="12"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="12"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="12"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="12"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="12"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="12"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="12"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="12"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="12"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="12"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="12"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="12"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="12"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="12"/>
     </row>
   </sheetData>
@@ -5402,18 +5397,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
         <v>110</v>
       </c>
@@ -5424,7 +5419,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="6" t="s">
         <v>11</v>
@@ -5441,7 +5436,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>111</v>
       </c>
@@ -5467,7 +5462,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>112</v>
       </c>
@@ -5486,7 +5481,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>113</v>
       </c>
@@ -5505,7 +5500,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D8" s="7"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -5513,7 +5508,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>114</v>
       </c>
@@ -5524,7 +5519,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="2:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>110</v>
       </c>
@@ -5538,7 +5533,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="6" t="s">
         <v>11</v>
@@ -5554,7 +5549,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>115</v>
       </c>
@@ -5572,7 +5567,7 @@
       <c r="H12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>116</v>
       </c>
@@ -5590,7 +5585,7 @@
       <c r="H13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>117</v>
       </c>
@@ -5608,14 +5603,14 @@
       <c r="H14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D15" s="7"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>118</v>
       </c>
@@ -5625,7 +5620,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>110</v>
       </c>
@@ -5638,7 +5633,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="6" t="s">
         <v>11</v>
@@ -5655,7 +5650,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>119</v>
       </c>
@@ -5674,7 +5669,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>120</v>
       </c>
@@ -5693,7 +5688,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>121</v>
       </c>
@@ -5712,7 +5707,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -5720,7 +5715,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -5728,7 +5723,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>122</v>
       </c>
@@ -5739,32 +5734,32 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="36" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="23" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="23" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="6" t="s">
         <v>50</v>
@@ -5776,7 +5771,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>73</v>
       </c>
@@ -5790,7 +5785,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>126</v>
       </c>
@@ -5804,7 +5799,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>71</v>
       </c>
@@ -5818,33 +5813,33 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F44" s="3"/>
     </row>
   </sheetData>
@@ -5861,19 +5856,19 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B3" s="51" t="s">
         <v>155</v>
       </c>
@@ -5926,7 +5921,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="52" t="s">
         <v>172</v>
       </c>
@@ -5975,7 +5970,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="52" t="s">
         <v>175</v>
       </c>
@@ -6024,7 +6019,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="52" t="s">
         <v>177</v>
       </c>
@@ -6075,7 +6070,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
         <v>179</v>
       </c>
@@ -6126,7 +6121,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="52" t="s">
         <v>181</v>
       </c>
@@ -6177,7 +6172,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="52" t="s">
         <v>183</v>
       </c>
@@ -6228,7 +6223,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="52" t="s">
         <v>184</v>
       </c>
@@ -6279,7 +6274,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
         <v>187</v>
       </c>
@@ -6330,7 +6325,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="52" t="s">
         <v>189</v>
       </c>
@@ -6381,7 +6376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
         <v>191</v>
       </c>
@@ -6432,7 +6427,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="52" t="s">
         <v>192</v>
       </c>
@@ -6483,7 +6478,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
         <v>194</v>
       </c>
@@ -6534,7 +6529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="52" t="s">
         <v>195</v>
       </c>
@@ -6585,7 +6580,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="52" t="s">
         <v>197</v>
       </c>
@@ -6636,7 +6631,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="52" t="s">
         <v>198</v>
       </c>
@@ -6687,7 +6682,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="52" t="s">
         <v>199</v>
       </c>
@@ -6738,7 +6733,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="52" t="s">
         <v>200</v>
       </c>
@@ -6789,7 +6784,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="52" t="s">
         <v>202</v>
       </c>
@@ -6840,7 +6835,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="52" t="s">
         <v>204</v>
       </c>
@@ -6885,7 +6880,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="52" t="s">
         <v>206</v>
       </c>
@@ -6932,7 +6927,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="52" t="s">
         <v>208</v>
       </c>
@@ -6992,9 +6987,9 @@
       <selection activeCell="B4" sqref="B4:R23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:21" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B3" s="51" t="s">
         <v>155</v>
       </c>
@@ -7056,7 +7051,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>172</v>
       </c>
@@ -7115,7 +7110,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>175</v>
       </c>
@@ -7174,7 +7169,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>177</v>
       </c>
@@ -7233,7 +7228,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>179</v>
       </c>
@@ -7292,7 +7287,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>181</v>
       </c>
@@ -7351,7 +7346,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>183</v>
       </c>
@@ -7410,7 +7405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>184</v>
       </c>
@@ -7469,7 +7464,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>187</v>
       </c>
@@ -7525,7 +7520,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>189</v>
       </c>
@@ -7581,7 +7576,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>191</v>
       </c>
@@ -7634,7 +7629,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>192</v>
       </c>
@@ -7690,7 +7685,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>194</v>
       </c>
@@ -7743,7 +7738,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>195</v>
       </c>
@@ -7799,7 +7794,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>197</v>
       </c>
@@ -7855,7 +7850,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>198</v>
       </c>
@@ -7914,7 +7909,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>199</v>
       </c>
@@ -7973,7 +7968,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>200</v>
       </c>
@@ -8032,7 +8027,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>202</v>
       </c>
@@ -8091,7 +8086,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>204</v>
       </c>
@@ -8150,7 +8145,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>206</v>
       </c>
@@ -8222,17 +8217,17 @@
       <selection activeCell="I4" sqref="I4:K69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="9:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="9:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="9:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="9:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I4" s="73" t="s">
         <v>217</v>
       </c>
       <c r="J4" s="74"/>
       <c r="K4" s="75"/>
     </row>
-    <row r="5" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I5" s="54" t="s">
         <v>50</v>
       </c>
@@ -8243,7 +8238,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I6" s="52" t="s">
         <v>218</v>
       </c>
@@ -8254,7 +8249,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I7" s="52" t="s">
         <v>218</v>
       </c>
@@ -8265,7 +8260,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I8" s="52" t="s">
         <v>218</v>
       </c>
@@ -8276,7 +8271,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I9" s="52" t="s">
         <v>218</v>
       </c>
@@ -8287,7 +8282,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I10" s="52" t="s">
         <v>218</v>
       </c>
@@ -8298,7 +8293,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I11" s="52" t="s">
         <v>218</v>
       </c>
@@ -8309,7 +8304,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I12" s="52" t="s">
         <v>218</v>
       </c>
@@ -8320,7 +8315,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I13" s="52" t="s">
         <v>218</v>
       </c>
@@ -8331,7 +8326,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I14" s="52" t="s">
         <v>218</v>
       </c>
@@ -8342,7 +8337,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I15" s="52" t="s">
         <v>218</v>
       </c>
@@ -8353,7 +8348,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I16" s="52" t="s">
         <v>218</v>
       </c>
@@ -8364,7 +8359,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I17" s="52" t="s">
         <v>218</v>
       </c>
@@ -8375,7 +8370,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I18" s="52" t="s">
         <v>218</v>
       </c>
@@ -8386,7 +8381,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I19" s="52" t="s">
         <v>218</v>
       </c>
@@ -8397,7 +8392,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I20" s="52" t="s">
         <v>218</v>
       </c>
@@ -8408,7 +8403,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I21" s="52" t="s">
         <v>218</v>
       </c>
@@ -8419,7 +8414,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I22" s="52" t="s">
         <v>227</v>
       </c>
@@ -8430,7 +8425,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I23" s="52" t="s">
         <v>227</v>
       </c>
@@ -8441,7 +8436,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I24" s="52" t="s">
         <v>227</v>
       </c>
@@ -8452,7 +8447,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I25" s="52" t="s">
         <v>227</v>
       </c>
@@ -8463,7 +8458,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I26" s="52" t="s">
         <v>227</v>
       </c>
@@ -8474,7 +8469,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I27" s="52" t="s">
         <v>227</v>
       </c>
@@ -8485,7 +8480,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I28" s="52" t="s">
         <v>227</v>
       </c>
@@ -8496,7 +8491,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I29" s="52" t="s">
         <v>227</v>
       </c>
@@ -8507,7 +8502,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="30" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I30" s="52" t="s">
         <v>227</v>
       </c>
@@ -8518,7 +8513,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I31" s="52" t="s">
         <v>227</v>
       </c>
@@ -8529,7 +8524,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="32" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I32" s="52" t="s">
         <v>227</v>
       </c>
@@ -8540,7 +8535,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I33" s="52" t="s">
         <v>227</v>
       </c>
@@ -8551,7 +8546,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I34" s="52" t="s">
         <v>227</v>
       </c>
@@ -8562,7 +8557,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I35" s="52" t="s">
         <v>227</v>
       </c>
@@ -8573,7 +8568,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I36" s="52" t="s">
         <v>227</v>
       </c>
@@ -8584,7 +8579,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I37" s="52" t="s">
         <v>227</v>
       </c>
@@ -8595,7 +8590,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I38" s="52" t="s">
         <v>228</v>
       </c>
@@ -8606,7 +8601,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I39" s="52" t="s">
         <v>228</v>
       </c>
@@ -8617,7 +8612,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I40" s="52" t="s">
         <v>228</v>
       </c>
@@ -8628,7 +8623,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I41" s="52" t="s">
         <v>228</v>
       </c>
@@ -8639,7 +8634,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I42" s="52" t="s">
         <v>228</v>
       </c>
@@ -8650,7 +8645,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I43" s="52" t="s">
         <v>228</v>
       </c>
@@ -8661,7 +8656,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="44" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I44" s="52" t="s">
         <v>228</v>
       </c>
@@ -8672,7 +8667,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="45" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I45" s="52" t="s">
         <v>228</v>
       </c>
@@ -8683,7 +8678,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="46" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I46" s="52" t="s">
         <v>228</v>
       </c>
@@ -8694,7 +8689,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I47" s="52" t="s">
         <v>228</v>
       </c>
@@ -8705,7 +8700,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I48" s="52" t="s">
         <v>228</v>
       </c>
@@ -8716,7 +8711,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I49" s="52" t="s">
         <v>228</v>
       </c>
@@ -8727,7 +8722,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I50" s="52" t="s">
         <v>228</v>
       </c>
@@ -8738,7 +8733,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I51" s="52" t="s">
         <v>228</v>
       </c>
@@ -8749,7 +8744,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="52" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I52" s="52" t="s">
         <v>228</v>
       </c>
@@ -8760,7 +8755,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="53" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I53" s="52" t="s">
         <v>228</v>
       </c>
@@ -8771,7 +8766,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="54" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I54" s="52" t="s">
         <v>229</v>
       </c>
@@ -8782,7 +8777,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I55" s="52" t="s">
         <v>229</v>
       </c>
@@ -8793,7 +8788,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I56" s="52" t="s">
         <v>229</v>
       </c>
@@ -8804,7 +8799,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="57" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I57" s="52" t="s">
         <v>229</v>
       </c>
@@ -8815,7 +8810,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="58" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I58" s="52" t="s">
         <v>229</v>
       </c>
@@ -8826,7 +8821,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="59" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I59" s="52" t="s">
         <v>229</v>
       </c>
@@ -8837,7 +8832,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I60" s="52" t="s">
         <v>229</v>
       </c>
@@ -8848,7 +8843,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I61" s="52" t="s">
         <v>229</v>
       </c>
@@ -8859,7 +8854,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I62" s="52" t="s">
         <v>229</v>
       </c>
@@ -8870,7 +8865,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I63" s="52" t="s">
         <v>229</v>
       </c>
@@ -8881,7 +8876,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="64" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I64" s="52" t="s">
         <v>229</v>
       </c>
@@ -8892,7 +8887,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="65" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I65" s="52" t="s">
         <v>229</v>
       </c>
@@ -8903,7 +8898,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="66" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I66" s="52" t="s">
         <v>229</v>
       </c>
@@ -8914,7 +8909,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I67" s="52" t="s">
         <v>229</v>
       </c>
@@ -8925,7 +8920,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="68" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I68" s="52" t="s">
         <v>229</v>
       </c>
@@ -8936,7 +8931,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="69" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I69" s="52" t="s">
         <v>229</v>
       </c>

</xml_diff>